<commit_message>
growth tweaks and some changes to preview loading
</commit_message>
<xml_diff>
--- a/src/lib/auto-complete/autocomplete_words.xlsx
+++ b/src/lib/auto-complete/autocomplete_words.xlsx
@@ -349,7 +349,7 @@
     <t>sand-jungle</t>
   </si>
   <si>
-    <t>range-[icon]</t>
+    <t>range-[replace_w_icon]</t>
   </si>
 </sst>
 </file>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C78" sqref="C3:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,54 +1470,54 @@
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B28" t="str">
         <f>A28</f>
-        <v>jungle-presence</v>
+        <v>jungle-mountain</v>
       </c>
       <c r="C28" t="str">
         <f>"{ label: """&amp;A28&amp;""", value: """&amp;B28&amp;""" },"</f>
-        <v>{ label: "jungle-presence", value: "jungle-presence" },</v>
+        <v>{ label: "jungle-mountain", value: "jungle-mountain" },</v>
       </c>
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B29" t="str">
         <f>A29</f>
-        <v>jungle-sand</v>
+        <v>jungle-presence</v>
       </c>
       <c r="C29" t="str">
         <f>"{ label: """&amp;A29&amp;""", value: """&amp;B29&amp;""" },"</f>
-        <v>{ label: "jungle-sand", value: "jungle-sand" },</v>
+        <v>{ label: "jungle-presence", value: "jungle-presence" },</v>
       </c>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" t="str">
         <f>A30</f>
-        <v>jungle-wetland</v>
+        <v>jungle-sand</v>
       </c>
       <c r="C30" t="str">
         <f>"{ label: """&amp;A30&amp;""", value: """&amp;B30&amp;""" },"</f>
-        <v>{ label: "jungle-wetland", value: "jungle-wetland" },</v>
+        <v>{ label: "jungle-sand", value: "jungle-sand" },</v>
       </c>
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B31" t="str">
         <f>A31</f>
-        <v>jungle-mountain</v>
+        <v>jungle-wetland</v>
       </c>
       <c r="C31" t="str">
         <f>"{ label: """&amp;A31&amp;""", value: """&amp;B31&amp;""" },"</f>
-        <v>{ label: "jungle-mountain", value: "jungle-mountain" },</v>
+        <v>{ label: "jungle-wetland", value: "jungle-wetland" },</v>
       </c>
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.25">
@@ -1799,11 +1799,11 @@
       </c>
       <c r="B53" t="str">
         <f>A53</f>
-        <v>range-[icon]</v>
+        <v>range-[replace_w_icon]</v>
       </c>
       <c r="C53" t="str">
         <f>"{ label: """&amp;A53&amp;""", value: """&amp;B53&amp;""" },"</f>
-        <v>{ label: "range-[icon]", value: "range-[icon]" },</v>
+        <v>{ label: "range-[replace_w_icon]", value: "range-[replace_w_icon]" },</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1899,15 +1899,15 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="B61" t="str">
         <f>A61</f>
-        <v>sand-presence</v>
+        <v>sand-jungle</v>
       </c>
       <c r="C61" t="str">
         <f>"{ label: """&amp;A61&amp;""", value: """&amp;B61&amp;""" },"</f>
-        <v>{ label: "sand-presence", value: "sand-presence" },</v>
+        <v>{ label: "sand-jungle", value: "sand-jungle" },</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1925,28 +1925,28 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B63" t="str">
         <f>A63</f>
-        <v>sand-wetland</v>
+        <v>sand-presence</v>
       </c>
       <c r="C63" t="str">
         <f>"{ label: """&amp;A63&amp;""", value: """&amp;B63&amp;""" },"</f>
-        <v>{ label: "sand-wetland", value: "sand-wetland" },</v>
+        <v>{ label: "sand-presence", value: "sand-presence" },</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="B64" t="str">
         <f>A64</f>
-        <v>sand-jungle</v>
+        <v>sand-wetland</v>
       </c>
       <c r="C64" t="str">
         <f>"{ label: """&amp;A64&amp;""", value: """&amp;B64&amp;""" },"</f>
-        <v>{ label: "sand-jungle", value: "sand-jungle" },</v>
+        <v>{ label: "sand-wetland", value: "sand-wetland" },</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2133,7 +2133,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:C2">
-    <sortState ref="A3:C74">
+    <sortState ref="A3:C78">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
modified to address neubee's concern
</commit_message>
<xml_diff>
--- a/src/lib/auto-complete/autocomplete_words.xlsx
+++ b/src/lib/auto-complete/autocomplete_words.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="growth" sheetId="1" r:id="rId1"/>
@@ -685,11 +685,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -712,12 +715,12 @@
         <v>4</v>
       </c>
       <c r="B3" t="str">
-        <f>A3&amp;"("</f>
-        <v>add-presence(</v>
+        <f>A3&amp;"()"</f>
+        <v>add-presence()</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C32" si="0">"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
-        <v>{ label: "add-presence", value: "add-presence(" },</v>
+        <v>{ label: "add-presence", value: "add-presence()" },</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,12 +728,12 @@
         <v>12</v>
       </c>
       <c r="B4" t="str">
-        <f>A4&amp;"("</f>
-        <v>add-token(</v>
+        <f t="shared" ref="B4:B6" si="1">A4&amp;"()"</f>
+        <v>add-token()</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "add-token", value: "add-token(" },</v>
+        <v>{ label: "add-token", value: "add-token()" },</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,12 +741,12 @@
         <v>24</v>
       </c>
       <c r="B5" t="str">
-        <f>A5&amp;"("</f>
-        <v>custom(</v>
+        <f t="shared" si="1"/>
+        <v>custom()</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "custom", value: "custom(" },</v>
+        <v>{ label: "custom", value: "custom()" },</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,12 +754,12 @@
         <v>22</v>
       </c>
       <c r="B6" t="str">
-        <f>A6&amp;"("</f>
-        <v>damage(</v>
+        <f t="shared" si="1"/>
+        <v>damage()</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "damage", value: "damage(" },</v>
+        <v>{ label: "damage", value: "damage()" },</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,12 +793,12 @@
         <v>20</v>
       </c>
       <c r="B9" t="str">
-        <f>A9&amp;"("</f>
-        <v>destroy-presence(</v>
+        <f t="shared" ref="B9:B10" si="2">A9&amp;"()"</f>
+        <v>destroy-presence()</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "destroy-presence", value: "destroy-presence(" },</v>
+        <v>{ label: "destroy-presence", value: "destroy-presence()" },</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -803,12 +806,12 @@
         <v>98</v>
       </c>
       <c r="B10" t="str">
-        <f>A10&amp;"("</f>
-        <v>discard(</v>
+        <f t="shared" si="2"/>
+        <v>discard()</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "discard", value: "discard(" },</v>
+        <v>{ label: "discard", value: "discard()" },</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -842,12 +845,12 @@
         <v>7</v>
       </c>
       <c r="B13" t="str">
-        <f>A13&amp;"("</f>
-        <v>element-marker(</v>
+        <f t="shared" ref="B13:B32" si="3">A13&amp;"()"</f>
+        <v>element-marker()</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "element-marker", value: "element-marker(" },</v>
+        <v>{ label: "element-marker", value: "element-marker()" },</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,12 +871,12 @@
         <v>21</v>
       </c>
       <c r="B15" t="str">
-        <f>A15&amp;"("</f>
-        <v>fear(</v>
+        <f t="shared" si="3"/>
+        <v>fear()</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "fear", value: "fear(" },</v>
+        <v>{ label: "fear", value: "fear()" },</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -894,12 +897,12 @@
         <v>15</v>
       </c>
       <c r="B17" t="str">
-        <f>A17&amp;"("</f>
-        <v>gain-card-play(</v>
+        <f t="shared" si="3"/>
+        <v>gain-card-play()</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "gain-card-play", value: "gain-card-play(" },</v>
+        <v>{ label: "gain-card-play", value: "gain-card-play()" },</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,12 +910,12 @@
         <v>6</v>
       </c>
       <c r="B18" t="str">
-        <f>A18&amp;"("</f>
-        <v>gain-element(</v>
+        <f t="shared" si="3"/>
+        <v>gain-element()</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "gain-element", value: "gain-element(" },</v>
+        <v>{ label: "gain-element", value: "gain-element()" },</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,12 +923,12 @@
         <v>3</v>
       </c>
       <c r="B19" t="str">
-        <f>A19&amp;"("</f>
-        <v>gain-energy(</v>
+        <f t="shared" si="3"/>
+        <v>gain-energy()</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "gain-energy", value: "gain-energy(" },</v>
+        <v>{ label: "gain-energy", value: "gain-energy()" },</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,12 +949,12 @@
         <v>18</v>
       </c>
       <c r="B21" t="str">
-        <f>A21&amp;"("</f>
-        <v>gain-range(</v>
+        <f t="shared" si="3"/>
+        <v>gain-range()</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "gain-range", value: "gain-range(" },</v>
+        <v>{ label: "gain-range", value: "gain-range()" },</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,12 +962,12 @@
         <v>9</v>
       </c>
       <c r="B22" t="str">
-        <f>A22&amp;"("</f>
-        <v>gather(</v>
+        <f t="shared" si="3"/>
+        <v>gather()</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "gather", value: "gather(" },</v>
+        <v>{ label: "gather", value: "gather()" },</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -985,12 +988,12 @@
         <v>97</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" ref="B24:B32" si="1">A24&amp;"("</f>
-        <v>incarna(</v>
+        <f t="shared" si="3"/>
+        <v>incarna()</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "incarna", value: "incarna(" },</v>
+        <v>{ label: "incarna", value: "incarna()" },</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,12 +1001,12 @@
         <v>19</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="1"/>
-        <v>isolate(</v>
+        <f t="shared" si="3"/>
+        <v>isolate()</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "isolate", value: "isolate(" },</v>
+        <v>{ label: "isolate", value: "isolate()" },</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,12 +1014,12 @@
         <v>23</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>make-fast(</v>
+        <f t="shared" si="3"/>
+        <v>make-fast()</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "make-fast", value: "make-fast(" },</v>
+        <v>{ label: "make-fast", value: "make-fast()" },</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,12 +1027,12 @@
         <v>10</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="1"/>
-        <v>move-presence(</v>
+        <f t="shared" si="3"/>
+        <v>move-presence()</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "move-presence", value: "move-presence(" },</v>
+        <v>{ label: "move-presence", value: "move-presence()" },</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1037,12 +1040,12 @@
         <v>25</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="1"/>
-        <v>or(</v>
+        <f t="shared" si="3"/>
+        <v>or()</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "or", value: "or(" },</v>
+        <v>{ label: "or", value: "or()" },</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1050,12 +1053,12 @@
         <v>26</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="1"/>
-        <v>presence-node(</v>
+        <f t="shared" si="3"/>
+        <v>presence-node()</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "presence-node", value: "presence-node(" },</v>
+        <v>{ label: "presence-node", value: "presence-node()" },</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,12 +1066,12 @@
         <v>8</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="1"/>
-        <v>push(</v>
+        <f t="shared" si="3"/>
+        <v>push()</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "push", value: "push(" },</v>
+        <v>{ label: "push", value: "push()" },</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1076,12 +1079,12 @@
         <v>5</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="1"/>
-        <v>reclaim(</v>
+        <f t="shared" si="3"/>
+        <v>reclaim()</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "reclaim", value: "reclaim(" },</v>
+        <v>{ label: "reclaim", value: "reclaim()" },</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,12 +1092,12 @@
         <v>99</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="1"/>
-        <v>replace(</v>
+        <f t="shared" si="3"/>
+        <v>replace()</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>{ label: "replace", value: "replace(" },</v>
+        <v>{ label: "replace", value: "replace()" },</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C78" sqref="C3:C78"/>
     </sheetView>
   </sheetViews>
@@ -1139,11 +1142,11 @@
         <v>45</v>
       </c>
       <c r="B3" t="str">
-        <f>A3</f>
+        <f t="shared" ref="B3:B34" si="0">A3</f>
         <v>air</v>
       </c>
       <c r="C3" t="str">
-        <f>"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
+        <f t="shared" ref="C3:C34" si="1">"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
         <v>{ label: "air", value: "air" },</v>
       </c>
     </row>
@@ -1152,11 +1155,11 @@
         <v>47</v>
       </c>
       <c r="B4" t="str">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>animal</v>
       </c>
       <c r="C4" t="str">
-        <f>"{ label: """&amp;A4&amp;""", value: """&amp;B4&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "animal", value: "animal" },</v>
       </c>
     </row>
@@ -1165,11 +1168,11 @@
         <v>33</v>
       </c>
       <c r="B5" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>any</v>
       </c>
       <c r="C5" t="str">
-        <f>"{ label: """&amp;A5&amp;""", value: """&amp;B5&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "any", value: "any" },</v>
       </c>
     </row>
@@ -1178,11 +1181,11 @@
         <v>66</v>
       </c>
       <c r="B6" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>badlands</v>
       </c>
       <c r="C6" t="str">
-        <f>"{ label: """&amp;A6&amp;""", value: """&amp;B6&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "badlands", value: "badlands" },</v>
       </c>
     </row>
@@ -1191,11 +1194,11 @@
         <v>62</v>
       </c>
       <c r="B7" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>beasts</v>
       </c>
       <c r="C7" t="str">
-        <f>"{ label: """&amp;A7&amp;""", value: """&amp;B7&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "beasts", value: "beasts" },</v>
       </c>
     </row>
@@ -1204,11 +1207,11 @@
         <v>50</v>
       </c>
       <c r="B8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>blight</v>
       </c>
       <c r="C8" t="str">
-        <f>"{ label: """&amp;A8&amp;""", value: """&amp;B8&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "blight", value: "blight" },</v>
       </c>
     </row>
@@ -1217,11 +1220,11 @@
         <v>39</v>
       </c>
       <c r="B9" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>city</v>
       </c>
       <c r="C9" t="str">
-        <f>"{ label: """&amp;A9&amp;""", value: """&amp;B9&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "city", value: "city" },</v>
       </c>
     </row>
@@ -1230,11 +1233,11 @@
         <v>93</v>
       </c>
       <c r="B10" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>custom1</v>
       </c>
       <c r="C10" t="str">
-        <f>"{ label: """&amp;A10&amp;""", value: """&amp;B10&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom1", value: "custom1" },</v>
       </c>
       <c r="E10" s="2"/>
@@ -1244,11 +1247,11 @@
         <v>94</v>
       </c>
       <c r="B11" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>custom2</v>
       </c>
       <c r="C11" t="str">
-        <f>"{ label: """&amp;A11&amp;""", value: """&amp;B11&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom2", value: "custom2" },</v>
       </c>
       <c r="E11" s="2"/>
@@ -1258,11 +1261,11 @@
         <v>95</v>
       </c>
       <c r="B12" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>custom3</v>
       </c>
       <c r="C12" t="str">
-        <f>"{ label: """&amp;A12&amp;""", value: """&amp;B12&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom3", value: "custom3" },</v>
       </c>
     </row>
@@ -1271,11 +1274,11 @@
         <v>96</v>
       </c>
       <c r="B13" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>custom4</v>
       </c>
       <c r="C13" t="str">
-        <f>"{ label: """&amp;A13&amp;""", value: """&amp;B13&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom4", value: "custom4" },</v>
       </c>
     </row>
@@ -1284,11 +1287,11 @@
         <v>61</v>
       </c>
       <c r="B14" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>dahan</v>
       </c>
       <c r="C14" t="str">
-        <f>"{ label: """&amp;A14&amp;""", value: """&amp;B14&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "dahan", value: "dahan" },</v>
       </c>
     </row>
@@ -1297,11 +1300,11 @@
         <v>57</v>
       </c>
       <c r="B15" t="str">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>destroyed-presence</v>
       </c>
       <c r="C15" t="str">
-        <f>"{ label: """&amp;A15&amp;""", value: """&amp;B15&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "destroyed-presence", value: "destroyed-presence" },</v>
       </c>
     </row>
@@ -1310,11 +1313,11 @@
         <v>64</v>
       </c>
       <c r="B16" t="str">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>disease</v>
       </c>
       <c r="C16" t="str">
-        <f>"{ label: """&amp;A16&amp;""", value: """&amp;B16&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "disease", value: "disease" },</v>
       </c>
     </row>
@@ -1323,11 +1326,11 @@
         <v>44</v>
       </c>
       <c r="B17" t="str">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>earth</v>
       </c>
       <c r="C17" t="str">
-        <f>"{ label: """&amp;A17&amp;""", value: """&amp;B17&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "earth", value: "earth" },</v>
       </c>
     </row>
@@ -1336,11 +1339,11 @@
         <v>37</v>
       </c>
       <c r="B18" t="str">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>explorer</v>
       </c>
       <c r="C18" t="str">
-        <f>"{ label: """&amp;A18&amp;""", value: """&amp;B18&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "explorer", value: "explorer" },</v>
       </c>
     </row>
@@ -1349,11 +1352,11 @@
         <v>52</v>
       </c>
       <c r="B19" t="str">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>fast</v>
       </c>
       <c r="C19" t="str">
-        <f>"{ label: """&amp;A19&amp;""", value: """&amp;B19&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "fast", value: "fast" },</v>
       </c>
       <c r="E19" s="2"/>
@@ -1363,11 +1366,11 @@
         <v>21</v>
       </c>
       <c r="B20" t="str">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>fear</v>
       </c>
       <c r="C20" t="str">
-        <f>"{ label: """&amp;A20&amp;""", value: """&amp;B20&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "fear", value: "fear" },</v>
       </c>
     </row>
@@ -1376,11 +1379,11 @@
         <v>32</v>
       </c>
       <c r="B21" t="str">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>fire</v>
       </c>
       <c r="C21" t="str">
-        <f>"{ label: """&amp;A21&amp;""", value: """&amp;B21&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "fire", value: "fire" },</v>
       </c>
     </row>
@@ -1389,11 +1392,11 @@
         <v>89</v>
       </c>
       <c r="B22" t="str">
-        <f>A22</f>
+        <f t="shared" si="0"/>
         <v>gain-range-1</v>
       </c>
       <c r="C22" t="str">
-        <f>"{ label: """&amp;A22&amp;""", value: """&amp;B22&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-1", value: "gain-range-1" },</v>
       </c>
     </row>
@@ -1402,11 +1405,11 @@
         <v>90</v>
       </c>
       <c r="B23" t="str">
-        <f>A23</f>
+        <f t="shared" si="0"/>
         <v>gain-range-2</v>
       </c>
       <c r="C23" t="str">
-        <f>"{ label: """&amp;A23&amp;""", value: """&amp;B23&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-2", value: "gain-range-2" },</v>
       </c>
       <c r="E23" s="2"/>
@@ -1421,11 +1424,11 @@
         <v>91</v>
       </c>
       <c r="B24" t="str">
-        <f>A24</f>
+        <f t="shared" si="0"/>
         <v>gain-range-3</v>
       </c>
       <c r="C24" t="str">
-        <f>"{ label: """&amp;A24&amp;""", value: """&amp;B24&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-3", value: "gain-range-3" },</v>
       </c>
     </row>
@@ -1434,11 +1437,11 @@
         <v>92</v>
       </c>
       <c r="B25" t="str">
-        <f>A25</f>
+        <f t="shared" si="0"/>
         <v>gain-range-x</v>
       </c>
       <c r="C25" t="str">
-        <f>"{ label: """&amp;A25&amp;""", value: """&amp;B25&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-x", value: "gain-range-x" },</v>
       </c>
     </row>
@@ -1447,11 +1450,11 @@
         <v>19</v>
       </c>
       <c r="B26" t="str">
-        <f>A26</f>
+        <f t="shared" si="0"/>
         <v>isolate</v>
       </c>
       <c r="C26" t="str">
-        <f>"{ label: """&amp;A26&amp;""", value: """&amp;B26&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "isolate", value: "isolate" },</v>
       </c>
     </row>
@@ -1460,11 +1463,11 @@
         <v>68</v>
       </c>
       <c r="B27" t="str">
-        <f>A27</f>
+        <f t="shared" si="0"/>
         <v>jungle</v>
       </c>
       <c r="C27" t="str">
-        <f>"{ label: """&amp;A27&amp;""", value: """&amp;B27&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle", value: "jungle" },</v>
       </c>
     </row>
@@ -1473,11 +1476,11 @@
         <v>103</v>
       </c>
       <c r="B28" t="str">
-        <f>A28</f>
+        <f t="shared" si="0"/>
         <v>jungle-mountain</v>
       </c>
       <c r="C28" t="str">
-        <f>"{ label: """&amp;A28&amp;""", value: """&amp;B28&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-mountain", value: "jungle-mountain" },</v>
       </c>
     </row>
@@ -1486,11 +1489,11 @@
         <v>85</v>
       </c>
       <c r="B29" t="str">
-        <f>A29</f>
+        <f t="shared" si="0"/>
         <v>jungle-presence</v>
       </c>
       <c r="C29" t="str">
-        <f>"{ label: """&amp;A29&amp;""", value: """&amp;B29&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-presence", value: "jungle-presence" },</v>
       </c>
     </row>
@@ -1499,11 +1502,11 @@
         <v>72</v>
       </c>
       <c r="B30" t="str">
-        <f>A30</f>
+        <f t="shared" si="0"/>
         <v>jungle-sand</v>
       </c>
       <c r="C30" t="str">
-        <f>"{ label: """&amp;A30&amp;""", value: """&amp;B30&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-sand", value: "jungle-sand" },</v>
       </c>
     </row>
@@ -1512,11 +1515,11 @@
         <v>71</v>
       </c>
       <c r="B31" t="str">
-        <f>A31</f>
+        <f t="shared" si="0"/>
         <v>jungle-wetland</v>
       </c>
       <c r="C31" t="str">
-        <f>"{ label: """&amp;A31&amp;""", value: """&amp;B31&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-wetland", value: "jungle-wetland" },</v>
       </c>
     </row>
@@ -1525,11 +1528,11 @@
         <v>79</v>
       </c>
       <c r="B32" t="str">
-        <f>A32</f>
+        <f t="shared" si="0"/>
         <v>major</v>
       </c>
       <c r="C32" t="str">
-        <f>"{ label: """&amp;A32&amp;""", value: """&amp;B32&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "major", value: "major" },</v>
       </c>
     </row>
@@ -1538,11 +1541,11 @@
         <v>36</v>
       </c>
       <c r="B33" t="str">
-        <f>A33</f>
+        <f t="shared" si="0"/>
         <v>markerminus</v>
       </c>
       <c r="C33" t="str">
-        <f>"{ label: """&amp;A33&amp;""", value: """&amp;B33&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "markerminus", value: "markerminus" },</v>
       </c>
     </row>
@@ -1551,11 +1554,11 @@
         <v>35</v>
       </c>
       <c r="B34" t="str">
-        <f>A34</f>
+        <f t="shared" si="0"/>
         <v>markerplus</v>
       </c>
       <c r="C34" t="str">
-        <f>"{ label: """&amp;A34&amp;""", value: """&amp;B34&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "markerplus", value: "markerplus" },</v>
       </c>
     </row>
@@ -1564,11 +1567,11 @@
         <v>78</v>
       </c>
       <c r="B35" t="str">
-        <f>A35</f>
+        <f t="shared" ref="B35:B66" si="2">A35</f>
         <v>minor</v>
       </c>
       <c r="C35" t="str">
-        <f>"{ label: """&amp;A35&amp;""", value: """&amp;B35&amp;""" },"</f>
+        <f t="shared" ref="C35:C66" si="3">"{ label: """&amp;A35&amp;""", value: """&amp;B35&amp;""" },"</f>
         <v>{ label: "minor", value: "minor" },</v>
       </c>
     </row>
@@ -1577,11 +1580,11 @@
         <v>49</v>
       </c>
       <c r="B36" t="str">
-        <f>A36</f>
+        <f t="shared" si="2"/>
         <v>moon</v>
       </c>
       <c r="C36" t="str">
-        <f>"{ label: """&amp;A36&amp;""", value: """&amp;B36&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "moon", value: "moon" },</v>
       </c>
     </row>
@@ -1590,11 +1593,11 @@
         <v>67</v>
       </c>
       <c r="B37" t="str">
-        <f>A37</f>
+        <f t="shared" si="2"/>
         <v>mountain</v>
       </c>
       <c r="C37" t="str">
-        <f>"{ label: """&amp;A37&amp;""", value: """&amp;B37&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain", value: "mountain" },</v>
       </c>
     </row>
@@ -1603,11 +1606,11 @@
         <v>74</v>
       </c>
       <c r="B38" t="str">
-        <f>A38</f>
+        <f t="shared" si="2"/>
         <v>mountain-jungle</v>
       </c>
       <c r="C38" t="str">
-        <f>"{ label: """&amp;A38&amp;""", value: """&amp;B38&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-jungle", value: "mountain-jungle" },</v>
       </c>
     </row>
@@ -1616,11 +1619,11 @@
         <v>87</v>
       </c>
       <c r="B39" t="str">
-        <f>A39</f>
+        <f t="shared" si="2"/>
         <v>mountain-presence</v>
       </c>
       <c r="C39" t="str">
-        <f>"{ label: """&amp;A39&amp;""", value: """&amp;B39&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-presence", value: "mountain-presence" },</v>
       </c>
     </row>
@@ -1629,11 +1632,11 @@
         <v>76</v>
       </c>
       <c r="B40" t="str">
-        <f>A40</f>
+        <f t="shared" si="2"/>
         <v>mountain-sand</v>
       </c>
       <c r="C40" t="str">
-        <f>"{ label: """&amp;A40&amp;""", value: """&amp;B40&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-sand", value: "mountain-sand" },</v>
       </c>
     </row>
@@ -1642,11 +1645,11 @@
         <v>75</v>
       </c>
       <c r="B41" t="str">
-        <f>A41</f>
+        <f t="shared" si="2"/>
         <v>mountain-wetland</v>
       </c>
       <c r="C41" t="str">
-        <f>"{ label: """&amp;A41&amp;""", value: """&amp;B41&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-wetland", value: "mountain-wetland" },</v>
       </c>
     </row>
@@ -1655,11 +1658,11 @@
         <v>41</v>
       </c>
       <c r="B42" t="str">
-        <f>A42</f>
+        <f t="shared" si="2"/>
         <v>move-presence-1</v>
       </c>
       <c r="C42" t="str">
-        <f>"{ label: """&amp;A42&amp;""", value: """&amp;B42&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-1", value: "move-presence-1" },</v>
       </c>
     </row>
@@ -1668,11 +1671,11 @@
         <v>58</v>
       </c>
       <c r="B43" t="str">
-        <f>A43</f>
+        <f t="shared" si="2"/>
         <v>move-presence-2</v>
       </c>
       <c r="C43" t="str">
-        <f>"{ label: """&amp;A43&amp;""", value: """&amp;B43&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-2", value: "move-presence-2" },</v>
       </c>
     </row>
@@ -1681,11 +1684,11 @@
         <v>59</v>
       </c>
       <c r="B44" t="str">
-        <f>A44</f>
+        <f t="shared" si="2"/>
         <v>move-presence-3</v>
       </c>
       <c r="C44" t="str">
-        <f>"{ label: """&amp;A44&amp;""", value: """&amp;B44&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-3", value: "move-presence-3" },</v>
       </c>
     </row>
@@ -1694,11 +1697,11 @@
         <v>60</v>
       </c>
       <c r="B45" t="str">
-        <f>A45</f>
+        <f t="shared" si="2"/>
         <v>move-presence-4</v>
       </c>
       <c r="C45" t="str">
-        <f>"{ label: """&amp;A45&amp;""", value: """&amp;B45&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-4", value: "move-presence-4" },</v>
       </c>
     </row>
@@ -1707,11 +1710,11 @@
         <v>56</v>
       </c>
       <c r="B46" t="str">
-        <f>A46</f>
+        <f t="shared" si="2"/>
         <v>no-own-presence</v>
       </c>
       <c r="C46" t="str">
-        <f>"{ label: """&amp;A46&amp;""", value: """&amp;B46&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "no-own-presence", value: "no-own-presence" },</v>
       </c>
     </row>
@@ -1720,11 +1723,11 @@
         <v>55</v>
       </c>
       <c r="B47" t="str">
-        <f>A47</f>
+        <f t="shared" si="2"/>
         <v>no-presence</v>
       </c>
       <c r="C47" t="str">
-        <f>"{ label: """&amp;A47&amp;""", value: """&amp;B47&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "no-presence", value: "no-presence" },</v>
       </c>
     </row>
@@ -1733,11 +1736,11 @@
         <v>70</v>
       </c>
       <c r="B48" t="str">
-        <f>A48</f>
+        <f t="shared" si="2"/>
         <v>ocean</v>
       </c>
       <c r="C48" t="str">
-        <f>"{ label: """&amp;A48&amp;""", value: """&amp;B48&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "ocean", value: "ocean" },</v>
       </c>
     </row>
@@ -1746,11 +1749,11 @@
         <v>25</v>
       </c>
       <c r="B49" t="str">
-        <f>A49</f>
+        <f t="shared" si="2"/>
         <v>or</v>
       </c>
       <c r="C49" t="str">
-        <f>"{ label: """&amp;A49&amp;""", value: """&amp;B49&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "or", value: "or" },</v>
       </c>
     </row>
@@ -1759,11 +1762,11 @@
         <v>46</v>
       </c>
       <c r="B50" t="str">
-        <f>A50</f>
+        <f t="shared" si="2"/>
         <v>plant</v>
       </c>
       <c r="C50" t="str">
-        <f>"{ label: """&amp;A50&amp;""", value: """&amp;B50&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "plant", value: "plant" },</v>
       </c>
     </row>
@@ -1772,11 +1775,11 @@
         <v>40</v>
       </c>
       <c r="B51" t="str">
-        <f>A51</f>
+        <f t="shared" si="2"/>
         <v>presence</v>
       </c>
       <c r="C51" t="str">
-        <f>"{ label: """&amp;A51&amp;""", value: """&amp;B51&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "presence", value: "presence" },</v>
       </c>
     </row>
@@ -1785,11 +1788,11 @@
         <v>53</v>
       </c>
       <c r="B52" t="str">
-        <f>A52</f>
+        <f t="shared" si="2"/>
         <v>range</v>
       </c>
       <c r="C52" t="str">
-        <f>"{ label: """&amp;A52&amp;""", value: """&amp;B52&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range", value: "range" },</v>
       </c>
     </row>
@@ -1798,11 +1801,11 @@
         <v>106</v>
       </c>
       <c r="B53" t="str">
-        <f>A53</f>
+        <f t="shared" si="2"/>
         <v>range-[replace_w_icon]</v>
       </c>
       <c r="C53" t="str">
-        <f>"{ label: """&amp;A53&amp;""", value: """&amp;B53&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-[replace_w_icon]", value: "range-[replace_w_icon]" },</v>
       </c>
     </row>
@@ -1811,11 +1814,11 @@
         <v>80</v>
       </c>
       <c r="B54" t="str">
-        <f>A54</f>
+        <f t="shared" si="2"/>
         <v>range-0</v>
       </c>
       <c r="C54" t="str">
-        <f>"{ label: """&amp;A54&amp;""", value: """&amp;B54&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-0", value: "range-0" },</v>
       </c>
     </row>
@@ -1824,11 +1827,11 @@
         <v>81</v>
       </c>
       <c r="B55" t="str">
-        <f>A55</f>
+        <f t="shared" si="2"/>
         <v>range-1</v>
       </c>
       <c r="C55" t="str">
-        <f>"{ label: """&amp;A55&amp;""", value: """&amp;B55&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-1", value: "range-1" },</v>
       </c>
     </row>
@@ -1837,11 +1840,11 @@
         <v>82</v>
       </c>
       <c r="B56" t="str">
-        <f>A56</f>
+        <f t="shared" si="2"/>
         <v>range-2</v>
       </c>
       <c r="C56" t="str">
-        <f>"{ label: """&amp;A56&amp;""", value: """&amp;B56&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-2", value: "range-2" },</v>
       </c>
     </row>
@@ -1850,11 +1853,11 @@
         <v>83</v>
       </c>
       <c r="B57" t="str">
-        <f>A57</f>
+        <f t="shared" si="2"/>
         <v>range-3</v>
       </c>
       <c r="C57" t="str">
-        <f>"{ label: """&amp;A57&amp;""", value: """&amp;B57&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-3", value: "range-3" },</v>
       </c>
     </row>
@@ -1863,11 +1866,11 @@
         <v>84</v>
       </c>
       <c r="B58" t="str">
-        <f>A58</f>
+        <f t="shared" si="2"/>
         <v>range-4</v>
       </c>
       <c r="C58" t="str">
-        <f>"{ label: """&amp;A58&amp;""", value: """&amp;B58&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-4", value: "range-4" },</v>
       </c>
     </row>
@@ -1876,11 +1879,11 @@
         <v>42</v>
       </c>
       <c r="B59" t="str">
-        <f>A59</f>
+        <f t="shared" si="2"/>
         <v>sacred-site</v>
       </c>
       <c r="C59" t="str">
-        <f>"{ label: """&amp;A59&amp;""", value: """&amp;B59&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sacred-site", value: "sacred-site" },</v>
       </c>
     </row>
@@ -1889,11 +1892,11 @@
         <v>51</v>
       </c>
       <c r="B60" t="str">
-        <f>A60</f>
+        <f t="shared" si="2"/>
         <v>sand</v>
       </c>
       <c r="C60" t="str">
-        <f>"{ label: """&amp;A60&amp;""", value: """&amp;B60&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand", value: "sand" },</v>
       </c>
     </row>
@@ -1902,11 +1905,11 @@
         <v>105</v>
       </c>
       <c r="B61" t="str">
-        <f>A61</f>
+        <f t="shared" si="2"/>
         <v>sand-jungle</v>
       </c>
       <c r="C61" t="str">
-        <f>"{ label: """&amp;A61&amp;""", value: """&amp;B61&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-jungle", value: "sand-jungle" },</v>
       </c>
     </row>
@@ -1915,11 +1918,11 @@
         <v>104</v>
       </c>
       <c r="B62" t="str">
-        <f>A62</f>
+        <f t="shared" si="2"/>
         <v>sand-mountain</v>
       </c>
       <c r="C62" t="str">
-        <f>"{ label: """&amp;A62&amp;""", value: """&amp;B62&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-mountain", value: "sand-mountain" },</v>
       </c>
     </row>
@@ -1928,11 +1931,11 @@
         <v>86</v>
       </c>
       <c r="B63" t="str">
-        <f>A63</f>
+        <f t="shared" si="2"/>
         <v>sand-presence</v>
       </c>
       <c r="C63" t="str">
-        <f>"{ label: """&amp;A63&amp;""", value: """&amp;B63&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-presence", value: "sand-presence" },</v>
       </c>
     </row>
@@ -1941,11 +1944,11 @@
         <v>73</v>
       </c>
       <c r="B64" t="str">
-        <f>A64</f>
+        <f t="shared" si="2"/>
         <v>sand-wetland</v>
       </c>
       <c r="C64" t="str">
-        <f>"{ label: """&amp;A64&amp;""", value: """&amp;B64&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-wetland", value: "sand-wetland" },</v>
       </c>
     </row>
@@ -1954,11 +1957,11 @@
         <v>77</v>
       </c>
       <c r="B65" t="str">
-        <f>A65</f>
+        <f t="shared" si="2"/>
         <v>slow</v>
       </c>
       <c r="C65" t="str">
-        <f>"{ label: """&amp;A65&amp;""", value: """&amp;B65&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "slow", value: "slow" },</v>
       </c>
     </row>
@@ -1967,11 +1970,11 @@
         <v>54</v>
       </c>
       <c r="B66" t="str">
-        <f>A66</f>
+        <f t="shared" si="2"/>
         <v>spirit</v>
       </c>
       <c r="C66" t="str">
-        <f>"{ label: """&amp;A66&amp;""", value: """&amp;B66&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "spirit", value: "spirit" },</v>
       </c>
     </row>
@@ -1980,11 +1983,11 @@
         <v>54</v>
       </c>
       <c r="B67" t="str">
-        <f>A67</f>
+        <f t="shared" ref="B67:B98" si="4">A67</f>
         <v>spirit</v>
       </c>
       <c r="C67" t="str">
-        <f>"{ label: """&amp;A67&amp;""", value: """&amp;B67&amp;""" },"</f>
+        <f t="shared" ref="C67:C98" si="5">"{ label: """&amp;A67&amp;""", value: """&amp;B67&amp;""" },"</f>
         <v>{ label: "spirit", value: "spirit" },</v>
       </c>
     </row>
@@ -1993,11 +1996,11 @@
         <v>34</v>
       </c>
       <c r="B68" t="str">
-        <f>A68</f>
+        <f t="shared" si="4"/>
         <v>star</v>
       </c>
       <c r="C68" t="str">
-        <f>"{ label: """&amp;A68&amp;""", value: """&amp;B68&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "star", value: "star" },</v>
       </c>
     </row>
@@ -2006,11 +2009,11 @@
         <v>65</v>
       </c>
       <c r="B69" t="str">
-        <f>A69</f>
+        <f t="shared" si="4"/>
         <v>strife</v>
       </c>
       <c r="C69" t="str">
-        <f>"{ label: """&amp;A69&amp;""", value: """&amp;B69&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "strife", value: "strife" },</v>
       </c>
     </row>
@@ -2019,11 +2022,11 @@
         <v>48</v>
       </c>
       <c r="B70" t="str">
-        <f>A70</f>
+        <f t="shared" si="4"/>
         <v>sun</v>
       </c>
       <c r="C70" t="str">
-        <f>"{ label: """&amp;A70&amp;""", value: """&amp;B70&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "sun", value: "sun" },</v>
       </c>
     </row>
@@ -2032,11 +2035,11 @@
         <v>100</v>
       </c>
       <c r="B71" t="str">
-        <f>A71</f>
+        <f t="shared" si="4"/>
         <v>terror-1</v>
       </c>
       <c r="C71" t="str">
-        <f>"{ label: """&amp;A71&amp;""", value: """&amp;B71&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "terror-1", value: "terror-1" },</v>
       </c>
     </row>
@@ -2045,11 +2048,11 @@
         <v>101</v>
       </c>
       <c r="B72" t="str">
-        <f>A72</f>
+        <f t="shared" si="4"/>
         <v>terror-2</v>
       </c>
       <c r="C72" t="str">
-        <f>"{ label: """&amp;A72&amp;""", value: """&amp;B72&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "terror-2", value: "terror-2" },</v>
       </c>
     </row>
@@ -2058,11 +2061,11 @@
         <v>102</v>
       </c>
       <c r="B73" t="str">
-        <f>A73</f>
+        <f t="shared" si="4"/>
         <v>terror-3</v>
       </c>
       <c r="C73" t="str">
-        <f>"{ label: """&amp;A73&amp;""", value: """&amp;B73&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "terror-3", value: "terror-3" },</v>
       </c>
     </row>
@@ -2071,11 +2074,11 @@
         <v>38</v>
       </c>
       <c r="B74" t="str">
-        <f>A74</f>
+        <f t="shared" si="4"/>
         <v>town</v>
       </c>
       <c r="C74" t="str">
-        <f>"{ label: """&amp;A74&amp;""", value: """&amp;B74&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "town", value: "town" },</v>
       </c>
     </row>
@@ -2084,11 +2087,11 @@
         <v>43</v>
       </c>
       <c r="B75" t="str">
-        <f>A75</f>
+        <f t="shared" si="4"/>
         <v>water</v>
       </c>
       <c r="C75" t="str">
-        <f>"{ label: """&amp;A75&amp;""", value: """&amp;B75&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "water", value: "water" },</v>
       </c>
     </row>
@@ -2097,11 +2100,11 @@
         <v>69</v>
       </c>
       <c r="B76" t="str">
-        <f>A76</f>
+        <f t="shared" si="4"/>
         <v>wetland</v>
       </c>
       <c r="C76" t="str">
-        <f>"{ label: """&amp;A76&amp;""", value: """&amp;B76&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "wetland", value: "wetland" },</v>
       </c>
     </row>
@@ -2110,11 +2113,11 @@
         <v>88</v>
       </c>
       <c r="B77" t="str">
-        <f>A77</f>
+        <f t="shared" si="4"/>
         <v>wetland-presence</v>
       </c>
       <c r="C77" t="str">
-        <f>"{ label: """&amp;A77&amp;""", value: """&amp;B77&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "wetland-presence", value: "wetland-presence" },</v>
       </c>
     </row>
@@ -2123,11 +2126,11 @@
         <v>63</v>
       </c>
       <c r="B78" t="str">
-        <f>A78</f>
+        <f t="shared" si="4"/>
         <v>wilds</v>
       </c>
       <c r="C78" t="str">
-        <f>"{ label: """&amp;A78&amp;""", value: """&amp;B78&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "wilds", value: "wilds" },</v>
       </c>
     </row>

</xml_diff>

<commit_message>
token + button fix
</commit_message>
<xml_diff>
--- a/src/lib/auto-complete/autocomplete_words.xlsx
+++ b/src/lib/auto-complete/autocomplete_words.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\spirit-island-builder\src\lib\auto-complete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\spirit-island-builder\src\lib\auto-complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="growth" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t>label</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>escalation</t>
+  </si>
+  <si>
+    <t>vitality</t>
+  </si>
+  <si>
+    <t>blank</t>
   </si>
 </sst>
 </file>
@@ -686,23 +692,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -713,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -722,11 +728,11 @@
         <v>add-presence()</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C32" si="0">"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
+        <f t="shared" ref="C3:C33" si="0">"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
         <v>{ label: "add-presence", value: "add-presence()" },</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -739,7 +745,7 @@
         <v>{ label: "add-token", value: "add-token()" },</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -752,7 +758,7 @@
         <v>{ label: "custom", value: "custom()" },</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -765,7 +771,7 @@
         <v>{ label: "damage", value: "damage()" },</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -778,7 +784,7 @@
         <v>{ label: "damage-1", value: "damage-1" },</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -791,7 +797,7 @@
         <v>{ label: "damage-2", value: "damage-2" },</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -804,7 +810,7 @@
         <v>{ label: "destroy-presence", value: "destroy-presence()" },</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -817,7 +823,7 @@
         <v>{ label: "discard", value: "discard()" },</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -830,7 +836,7 @@
         <v>{ label: "discard-card", value: "discard-card" },</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -843,12 +849,12 @@
         <v>{ label: "discard-cards", value: "discard-cards" },</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" ref="B13:B32" si="3">A13&amp;"()"</f>
+        <f t="shared" ref="B13:B33" si="3">A13&amp;"()"</f>
         <v>element-marker()</v>
       </c>
       <c r="C13" t="str">
@@ -856,7 +862,7 @@
         <v>{ label: "element-marker", value: "element-marker()" },</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -869,7 +875,7 @@
         <v>{ label: "energy-per-play", value: "energy-per-play" },</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -882,7 +888,7 @@
         <v>{ label: "fear", value: "fear()" },</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -895,7 +901,7 @@
         <v>{ label: "forget-power-card", value: "forget-power-card" },</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -908,7 +914,7 @@
         <v>{ label: "gain-card-play", value: "gain-card-play()" },</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -921,7 +927,7 @@
         <v>{ label: "gain-element", value: "gain-element()" },</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -934,7 +940,7 @@
         <v>{ label: "gain-energy", value: "gain-energy()" },</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -947,7 +953,7 @@
         <v>{ label: "gain-power-card", value: "gain-power-card" },</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -960,7 +966,7 @@
         <v>{ label: "gain-range", value: "gain-range()" },</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -973,7 +979,7 @@
         <v>{ label: "gather", value: "gather()" },</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -986,7 +992,7 @@
         <v>{ label: "ignore-range", value: "ignore-range" },</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>{ label: "incarna", value: "incarna()" },</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>{ label: "isolate", value: "isolate()" },</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>{ label: "make-fast", value: "make-fast()" },</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>{ label: "move-presence", value: "move-presence()" },</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>{ label: "or", value: "or()" },</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>{ label: "presence-node", value: "presence-node()" },</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>{ label: "push", value: "push()" },</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>{ label: "reclaim", value: "reclaim()" },</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -1101,6 +1107,19 @@
       <c r="C32" t="str">
         <f t="shared" si="0"/>
         <v>{ label: "replace", value: "replace()" },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="3"/>
+        <v>blank()</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>{ label: "blank", value: "blank()" },</v>
       </c>
     </row>
   </sheetData>
@@ -1116,20 +1135,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR79"/>
+  <dimension ref="A1:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C79"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1140,279 +1159,279 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="str">
-        <f>A3</f>
+        <f t="shared" ref="B3:B34" si="0">A3</f>
         <v>air</v>
       </c>
       <c r="C3" t="str">
-        <f>"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
+        <f t="shared" ref="C3:C34" si="1">"{ label: """&amp;A3&amp;""", value: """&amp;B3&amp;""" },"</f>
         <v>{ label: "air", value: "air" },</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="str">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>animal</v>
       </c>
       <c r="C4" t="str">
-        <f>"{ label: """&amp;A4&amp;""", value: """&amp;B4&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "animal", value: "animal" },</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>any</v>
       </c>
       <c r="C5" t="str">
-        <f>"{ label: """&amp;A5&amp;""", value: """&amp;B5&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "any", value: "any" },</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
       <c r="B6" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>badlands</v>
       </c>
       <c r="C6" t="str">
-        <f>"{ label: """&amp;A6&amp;""", value: """&amp;B6&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "badlands", value: "badlands" },</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
       <c r="B7" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>beasts</v>
       </c>
       <c r="C7" t="str">
-        <f>"{ label: """&amp;A7&amp;""", value: """&amp;B7&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "beasts", value: "beasts" },</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>blight</v>
       </c>
       <c r="C8" t="str">
-        <f>"{ label: """&amp;A8&amp;""", value: """&amp;B8&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "blight", value: "blight" },</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>39</v>
       </c>
       <c r="B9" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>city</v>
       </c>
       <c r="C9" t="str">
-        <f>"{ label: """&amp;A9&amp;""", value: """&amp;B9&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "city", value: "city" },</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>93</v>
       </c>
       <c r="B10" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>custom1</v>
       </c>
       <c r="C10" t="str">
-        <f>"{ label: """&amp;A10&amp;""", value: """&amp;B10&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom1", value: "custom1" },</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>94</v>
       </c>
       <c r="B11" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>custom2</v>
       </c>
       <c r="C11" t="str">
-        <f>"{ label: """&amp;A11&amp;""", value: """&amp;B11&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom2", value: "custom2" },</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>95</v>
       </c>
       <c r="B12" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>custom3</v>
       </c>
       <c r="C12" t="str">
-        <f>"{ label: """&amp;A12&amp;""", value: """&amp;B12&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom3", value: "custom3" },</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>96</v>
       </c>
       <c r="B13" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>custom4</v>
       </c>
       <c r="C13" t="str">
-        <f>"{ label: """&amp;A13&amp;""", value: """&amp;B13&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "custom4", value: "custom4" },</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>61</v>
       </c>
       <c r="B14" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>dahan</v>
       </c>
       <c r="C14" t="str">
-        <f>"{ label: """&amp;A14&amp;""", value: """&amp;B14&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "dahan", value: "dahan" },</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>57</v>
       </c>
       <c r="B15" t="str">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>destroyed-presence</v>
       </c>
       <c r="C15" t="str">
-        <f>"{ label: """&amp;A15&amp;""", value: """&amp;B15&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "destroyed-presence", value: "destroyed-presence" },</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>64</v>
       </c>
       <c r="B16" t="str">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>disease</v>
       </c>
       <c r="C16" t="str">
-        <f>"{ label: """&amp;A16&amp;""", value: """&amp;B16&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "disease", value: "disease" },</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>44</v>
       </c>
       <c r="B17" t="str">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>earth</v>
       </c>
       <c r="C17" t="str">
-        <f>"{ label: """&amp;A17&amp;""", value: """&amp;B17&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "earth", value: "earth" },</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>107</v>
       </c>
       <c r="B18" t="str">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>escalation</v>
       </c>
       <c r="C18" t="str">
-        <f>"{ label: """&amp;A18&amp;""", value: """&amp;B18&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "escalation", value: "escalation" },</v>
       </c>
     </row>
-    <row r="19" spans="1:44" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="str">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>explorer</v>
       </c>
       <c r="C19" t="str">
-        <f>"{ label: """&amp;A19&amp;""", value: """&amp;B19&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "explorer", value: "explorer" },</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="str">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>fast</v>
       </c>
       <c r="C20" t="str">
-        <f>"{ label: """&amp;A20&amp;""", value: """&amp;B20&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "fast", value: "fast" },</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="str">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>fear</v>
       </c>
       <c r="C21" t="str">
-        <f>"{ label: """&amp;A21&amp;""", value: """&amp;B21&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "fear", value: "fear" },</v>
       </c>
     </row>
-    <row r="22" spans="1:44" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B22" t="str">
-        <f>A22</f>
+        <f t="shared" si="0"/>
         <v>fire</v>
       </c>
       <c r="C22" t="str">
-        <f>"{ label: """&amp;A22&amp;""", value: """&amp;B22&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "fire", value: "fire" },</v>
       </c>
     </row>
-    <row r="23" spans="1:44" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>89</v>
       </c>
       <c r="B23" t="str">
-        <f>A23</f>
+        <f t="shared" si="0"/>
         <v>gain-range-1</v>
       </c>
       <c r="C23" t="str">
-        <f>"{ label: """&amp;A23&amp;""", value: """&amp;B23&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-1", value: "gain-range-1" },</v>
       </c>
       <c r="E23" s="2"/>
@@ -1422,732 +1441,745 @@
       <c r="AG23" s="2"/>
       <c r="AR23" s="2"/>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>90</v>
       </c>
       <c r="B24" t="str">
-        <f>A24</f>
+        <f t="shared" si="0"/>
         <v>gain-range-2</v>
       </c>
       <c r="C24" t="str">
-        <f>"{ label: """&amp;A24&amp;""", value: """&amp;B24&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-2", value: "gain-range-2" },</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
       <c r="B25" t="str">
-        <f>A25</f>
+        <f t="shared" si="0"/>
         <v>gain-range-3</v>
       </c>
       <c r="C25" t="str">
-        <f>"{ label: """&amp;A25&amp;""", value: """&amp;B25&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-3", value: "gain-range-3" },</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>92</v>
       </c>
       <c r="B26" t="str">
-        <f>A26</f>
+        <f t="shared" si="0"/>
         <v>gain-range-x</v>
       </c>
       <c r="C26" t="str">
-        <f>"{ label: """&amp;A26&amp;""", value: """&amp;B26&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "gain-range-x", value: "gain-range-x" },</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>19</v>
       </c>
       <c r="B27" t="str">
-        <f>A27</f>
+        <f t="shared" si="0"/>
         <v>isolate</v>
       </c>
       <c r="C27" t="str">
-        <f>"{ label: """&amp;A27&amp;""", value: """&amp;B27&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "isolate", value: "isolate" },</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>68</v>
       </c>
       <c r="B28" t="str">
-        <f>A28</f>
+        <f t="shared" si="0"/>
         <v>jungle</v>
       </c>
       <c r="C28" t="str">
-        <f>"{ label: """&amp;A28&amp;""", value: """&amp;B28&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle", value: "jungle" },</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>103</v>
       </c>
       <c r="B29" t="str">
-        <f>A29</f>
+        <f t="shared" si="0"/>
         <v>jungle-mountain</v>
       </c>
       <c r="C29" t="str">
-        <f>"{ label: """&amp;A29&amp;""", value: """&amp;B29&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-mountain", value: "jungle-mountain" },</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>85</v>
       </c>
       <c r="B30" t="str">
-        <f>A30</f>
+        <f t="shared" si="0"/>
         <v>jungle-presence</v>
       </c>
       <c r="C30" t="str">
-        <f>"{ label: """&amp;A30&amp;""", value: """&amp;B30&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-presence", value: "jungle-presence" },</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>72</v>
       </c>
       <c r="B31" t="str">
-        <f>A31</f>
+        <f t="shared" si="0"/>
         <v>jungle-sand</v>
       </c>
       <c r="C31" t="str">
-        <f>"{ label: """&amp;A31&amp;""", value: """&amp;B31&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-sand", value: "jungle-sand" },</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>71</v>
       </c>
       <c r="B32" t="str">
-        <f>A32</f>
+        <f t="shared" si="0"/>
         <v>jungle-wetland</v>
       </c>
       <c r="C32" t="str">
-        <f>"{ label: """&amp;A32&amp;""", value: """&amp;B32&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "jungle-wetland", value: "jungle-wetland" },</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>79</v>
       </c>
       <c r="B33" t="str">
-        <f>A33</f>
+        <f t="shared" si="0"/>
         <v>major</v>
       </c>
       <c r="C33" t="str">
-        <f>"{ label: """&amp;A33&amp;""", value: """&amp;B33&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "major", value: "major" },</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34" t="str">
-        <f>A34</f>
+        <f t="shared" si="0"/>
         <v>markerminus</v>
       </c>
       <c r="C34" t="str">
-        <f>"{ label: """&amp;A34&amp;""", value: """&amp;B34&amp;""" },"</f>
+        <f t="shared" si="1"/>
         <v>{ label: "markerminus", value: "markerminus" },</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="str">
-        <f>A35</f>
+        <f t="shared" ref="B35:B66" si="2">A35</f>
         <v>markerplus</v>
       </c>
       <c r="C35" t="str">
-        <f>"{ label: """&amp;A35&amp;""", value: """&amp;B35&amp;""" },"</f>
+        <f t="shared" ref="C35:C66" si="3">"{ label: """&amp;A35&amp;""", value: """&amp;B35&amp;""" },"</f>
         <v>{ label: "markerplus", value: "markerplus" },</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>78</v>
       </c>
       <c r="B36" t="str">
-        <f>A36</f>
+        <f t="shared" si="2"/>
         <v>minor</v>
       </c>
       <c r="C36" t="str">
-        <f>"{ label: """&amp;A36&amp;""", value: """&amp;B36&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "minor", value: "minor" },</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>49</v>
       </c>
       <c r="B37" t="str">
-        <f>A37</f>
+        <f t="shared" si="2"/>
         <v>moon</v>
       </c>
       <c r="C37" t="str">
-        <f>"{ label: """&amp;A37&amp;""", value: """&amp;B37&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "moon", value: "moon" },</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>67</v>
       </c>
       <c r="B38" t="str">
-        <f>A38</f>
+        <f t="shared" si="2"/>
         <v>mountain</v>
       </c>
       <c r="C38" t="str">
-        <f>"{ label: """&amp;A38&amp;""", value: """&amp;B38&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain", value: "mountain" },</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
       <c r="B39" t="str">
-        <f>A39</f>
+        <f t="shared" si="2"/>
         <v>mountain-jungle</v>
       </c>
       <c r="C39" t="str">
-        <f>"{ label: """&amp;A39&amp;""", value: """&amp;B39&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-jungle", value: "mountain-jungle" },</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>87</v>
       </c>
       <c r="B40" t="str">
-        <f>A40</f>
+        <f t="shared" si="2"/>
         <v>mountain-presence</v>
       </c>
       <c r="C40" t="str">
-        <f>"{ label: """&amp;A40&amp;""", value: """&amp;B40&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-presence", value: "mountain-presence" },</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>76</v>
       </c>
       <c r="B41" t="str">
-        <f>A41</f>
+        <f t="shared" si="2"/>
         <v>mountain-sand</v>
       </c>
       <c r="C41" t="str">
-        <f>"{ label: """&amp;A41&amp;""", value: """&amp;B41&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-sand", value: "mountain-sand" },</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>75</v>
       </c>
       <c r="B42" t="str">
-        <f>A42</f>
+        <f t="shared" si="2"/>
         <v>mountain-wetland</v>
       </c>
       <c r="C42" t="str">
-        <f>"{ label: """&amp;A42&amp;""", value: """&amp;B42&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "mountain-wetland", value: "mountain-wetland" },</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="str">
-        <f>A43</f>
+        <f t="shared" si="2"/>
         <v>move-presence-1</v>
       </c>
       <c r="C43" t="str">
-        <f>"{ label: """&amp;A43&amp;""", value: """&amp;B43&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-1", value: "move-presence-1" },</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
       <c r="B44" t="str">
-        <f>A44</f>
+        <f t="shared" si="2"/>
         <v>move-presence-2</v>
       </c>
       <c r="C44" t="str">
-        <f>"{ label: """&amp;A44&amp;""", value: """&amp;B44&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-2", value: "move-presence-2" },</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
       <c r="B45" t="str">
-        <f>A45</f>
+        <f t="shared" si="2"/>
         <v>move-presence-3</v>
       </c>
       <c r="C45" t="str">
-        <f>"{ label: """&amp;A45&amp;""", value: """&amp;B45&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-3", value: "move-presence-3" },</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
       <c r="B46" t="str">
-        <f>A46</f>
+        <f t="shared" si="2"/>
         <v>move-presence-4</v>
       </c>
       <c r="C46" t="str">
-        <f>"{ label: """&amp;A46&amp;""", value: """&amp;B46&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "move-presence-4", value: "move-presence-4" },</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>56</v>
       </c>
       <c r="B47" t="str">
-        <f>A47</f>
+        <f t="shared" si="2"/>
         <v>no-own-presence</v>
       </c>
       <c r="C47" t="str">
-        <f>"{ label: """&amp;A47&amp;""", value: """&amp;B47&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "no-own-presence", value: "no-own-presence" },</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>55</v>
       </c>
       <c r="B48" t="str">
-        <f>A48</f>
+        <f t="shared" si="2"/>
         <v>no-presence</v>
       </c>
       <c r="C48" t="str">
-        <f>"{ label: """&amp;A48&amp;""", value: """&amp;B48&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "no-presence", value: "no-presence" },</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>70</v>
       </c>
       <c r="B49" t="str">
-        <f>A49</f>
+        <f t="shared" si="2"/>
         <v>ocean</v>
       </c>
       <c r="C49" t="str">
-        <f>"{ label: """&amp;A49&amp;""", value: """&amp;B49&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "ocean", value: "ocean" },</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>25</v>
       </c>
       <c r="B50" t="str">
-        <f>A50</f>
+        <f t="shared" si="2"/>
         <v>or</v>
       </c>
       <c r="C50" t="str">
-        <f>"{ label: """&amp;A50&amp;""", value: """&amp;B50&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "or", value: "or" },</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>46</v>
       </c>
       <c r="B51" t="str">
-        <f>A51</f>
+        <f t="shared" si="2"/>
         <v>plant</v>
       </c>
       <c r="C51" t="str">
-        <f>"{ label: """&amp;A51&amp;""", value: """&amp;B51&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "plant", value: "plant" },</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>40</v>
       </c>
       <c r="B52" t="str">
-        <f>A52</f>
+        <f t="shared" si="2"/>
         <v>presence</v>
       </c>
       <c r="C52" t="str">
-        <f>"{ label: """&amp;A52&amp;""", value: """&amp;B52&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "presence", value: "presence" },</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="str">
-        <f>A53</f>
+        <f t="shared" si="2"/>
         <v>range</v>
       </c>
       <c r="C53" t="str">
-        <f>"{ label: """&amp;A53&amp;""", value: """&amp;B53&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range", value: "range" },</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>106</v>
       </c>
       <c r="B54" t="str">
-        <f>A54</f>
+        <f t="shared" si="2"/>
         <v>range-[replace_w_icon]</v>
       </c>
       <c r="C54" t="str">
-        <f>"{ label: """&amp;A54&amp;""", value: """&amp;B54&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-[replace_w_icon]", value: "range-[replace_w_icon]" },</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>80</v>
       </c>
       <c r="B55" t="str">
-        <f>A55</f>
+        <f t="shared" si="2"/>
         <v>range-0</v>
       </c>
       <c r="C55" t="str">
-        <f>"{ label: """&amp;A55&amp;""", value: """&amp;B55&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-0", value: "range-0" },</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>81</v>
       </c>
       <c r="B56" t="str">
-        <f>A56</f>
+        <f t="shared" si="2"/>
         <v>range-1</v>
       </c>
       <c r="C56" t="str">
-        <f>"{ label: """&amp;A56&amp;""", value: """&amp;B56&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-1", value: "range-1" },</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>82</v>
       </c>
       <c r="B57" t="str">
-        <f>A57</f>
+        <f t="shared" si="2"/>
         <v>range-2</v>
       </c>
       <c r="C57" t="str">
-        <f>"{ label: """&amp;A57&amp;""", value: """&amp;B57&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-2", value: "range-2" },</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>83</v>
       </c>
       <c r="B58" t="str">
-        <f>A58</f>
+        <f t="shared" si="2"/>
         <v>range-3</v>
       </c>
       <c r="C58" t="str">
-        <f>"{ label: """&amp;A58&amp;""", value: """&amp;B58&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-3", value: "range-3" },</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>84</v>
       </c>
       <c r="B59" t="str">
-        <f>A59</f>
+        <f t="shared" si="2"/>
         <v>range-4</v>
       </c>
       <c r="C59" t="str">
-        <f>"{ label: """&amp;A59&amp;""", value: """&amp;B59&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "range-4", value: "range-4" },</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>42</v>
       </c>
       <c r="B60" t="str">
-        <f>A60</f>
+        <f t="shared" si="2"/>
         <v>sacred-site</v>
       </c>
       <c r="C60" t="str">
-        <f>"{ label: """&amp;A60&amp;""", value: """&amp;B60&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sacred-site", value: "sacred-site" },</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>51</v>
       </c>
       <c r="B61" t="str">
-        <f>A61</f>
+        <f t="shared" si="2"/>
         <v>sand</v>
       </c>
       <c r="C61" t="str">
-        <f>"{ label: """&amp;A61&amp;""", value: """&amp;B61&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand", value: "sand" },</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>105</v>
       </c>
       <c r="B62" t="str">
-        <f>A62</f>
+        <f t="shared" si="2"/>
         <v>sand-jungle</v>
       </c>
       <c r="C62" t="str">
-        <f>"{ label: """&amp;A62&amp;""", value: """&amp;B62&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-jungle", value: "sand-jungle" },</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>104</v>
       </c>
       <c r="B63" t="str">
-        <f>A63</f>
+        <f t="shared" si="2"/>
         <v>sand-mountain</v>
       </c>
       <c r="C63" t="str">
-        <f>"{ label: """&amp;A63&amp;""", value: """&amp;B63&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-mountain", value: "sand-mountain" },</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>86</v>
       </c>
       <c r="B64" t="str">
-        <f>A64</f>
+        <f t="shared" si="2"/>
         <v>sand-presence</v>
       </c>
       <c r="C64" t="str">
-        <f>"{ label: """&amp;A64&amp;""", value: """&amp;B64&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-presence", value: "sand-presence" },</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
       <c r="B65" t="str">
-        <f>A65</f>
+        <f t="shared" si="2"/>
         <v>sand-wetland</v>
       </c>
       <c r="C65" t="str">
-        <f>"{ label: """&amp;A65&amp;""", value: """&amp;B65&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "sand-wetland", value: "sand-wetland" },</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>77</v>
       </c>
       <c r="B66" t="str">
-        <f>A66</f>
+        <f t="shared" si="2"/>
         <v>slow</v>
       </c>
       <c r="C66" t="str">
-        <f>"{ label: """&amp;A66&amp;""", value: """&amp;B66&amp;""" },"</f>
+        <f t="shared" si="3"/>
         <v>{ label: "slow", value: "slow" },</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>54</v>
       </c>
       <c r="B67" t="str">
-        <f>A67</f>
+        <f t="shared" ref="B67:B98" si="4">A67</f>
         <v>spirit</v>
       </c>
       <c r="C67" t="str">
-        <f>"{ label: """&amp;A67&amp;""", value: """&amp;B67&amp;""" },"</f>
+        <f t="shared" ref="C67:C98" si="5">"{ label: """&amp;A67&amp;""", value: """&amp;B67&amp;""" },"</f>
         <v>{ label: "spirit", value: "spirit" },</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>54</v>
       </c>
       <c r="B68" t="str">
-        <f>A68</f>
+        <f t="shared" si="4"/>
         <v>spirit</v>
       </c>
       <c r="C68" t="str">
-        <f>"{ label: """&amp;A68&amp;""", value: """&amp;B68&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "spirit", value: "spirit" },</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>34</v>
       </c>
       <c r="B69" t="str">
-        <f>A69</f>
+        <f t="shared" si="4"/>
         <v>star</v>
       </c>
       <c r="C69" t="str">
-        <f>"{ label: """&amp;A69&amp;""", value: """&amp;B69&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "star", value: "star" },</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>65</v>
       </c>
       <c r="B70" t="str">
-        <f>A70</f>
+        <f t="shared" si="4"/>
         <v>strife</v>
       </c>
       <c r="C70" t="str">
-        <f>"{ label: """&amp;A70&amp;""", value: """&amp;B70&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "strife", value: "strife" },</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>48</v>
       </c>
       <c r="B71" t="str">
-        <f>A71</f>
+        <f t="shared" si="4"/>
         <v>sun</v>
       </c>
       <c r="C71" t="str">
-        <f>"{ label: """&amp;A71&amp;""", value: """&amp;B71&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "sun", value: "sun" },</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>100</v>
       </c>
       <c r="B72" t="str">
-        <f>A72</f>
+        <f t="shared" si="4"/>
         <v>terror-1</v>
       </c>
       <c r="C72" t="str">
-        <f>"{ label: """&amp;A72&amp;""", value: """&amp;B72&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "terror-1", value: "terror-1" },</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>101</v>
       </c>
       <c r="B73" t="str">
-        <f>A73</f>
+        <f t="shared" si="4"/>
         <v>terror-2</v>
       </c>
       <c r="C73" t="str">
-        <f>"{ label: """&amp;A73&amp;""", value: """&amp;B73&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "terror-2", value: "terror-2" },</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>102</v>
       </c>
       <c r="B74" t="str">
-        <f>A74</f>
+        <f t="shared" si="4"/>
         <v>terror-3</v>
       </c>
       <c r="C74" t="str">
-        <f>"{ label: """&amp;A74&amp;""", value: """&amp;B74&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "terror-3", value: "terror-3" },</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>38</v>
       </c>
       <c r="B75" t="str">
-        <f>A75</f>
+        <f t="shared" si="4"/>
         <v>town</v>
       </c>
       <c r="C75" t="str">
-        <f>"{ label: """&amp;A75&amp;""", value: """&amp;B75&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "town", value: "town" },</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>43</v>
       </c>
       <c r="B76" t="str">
-        <f>A76</f>
+        <f t="shared" si="4"/>
         <v>water</v>
       </c>
       <c r="C76" t="str">
-        <f>"{ label: """&amp;A76&amp;""", value: """&amp;B76&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "water", value: "water" },</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>69</v>
       </c>
       <c r="B77" t="str">
-        <f>A77</f>
+        <f t="shared" si="4"/>
         <v>wetland</v>
       </c>
       <c r="C77" t="str">
-        <f>"{ label: """&amp;A77&amp;""", value: """&amp;B77&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "wetland", value: "wetland" },</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>88</v>
       </c>
       <c r="B78" t="str">
-        <f>A78</f>
+        <f t="shared" si="4"/>
         <v>wetland-presence</v>
       </c>
       <c r="C78" t="str">
-        <f>"{ label: """&amp;A78&amp;""", value: """&amp;B78&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "wetland-presence", value: "wetland-presence" },</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>63</v>
       </c>
       <c r="B79" t="str">
-        <f>A79</f>
+        <f t="shared" si="4"/>
         <v>wilds</v>
       </c>
       <c r="C79" t="str">
-        <f>"{ label: """&amp;A79&amp;""", value: """&amp;B79&amp;""" },"</f>
+        <f t="shared" si="5"/>
         <v>{ label: "wilds", value: "wilds" },</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="4"/>
+        <v>vitality</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="5"/>
+        <v>{ label: "vitality", value: "vitality" },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>